<commit_message>
Session (Admin) and Roles
</commit_message>
<xml_diff>
--- a/Moqup/Iconos.xlsx
+++ b/Moqup/Iconos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GamerNest\Moqup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC91712D-84D6-4E94-A102-E06AE6A45A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1566B1-79C8-436E-9B5B-158D3384C379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>MENÚ LATERAL</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>https://fontawesome.com/icons/bars?s=solid&amp;f=classic</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>right-from-bracket</t>
+  </si>
+  <si>
+    <t>https://fontawesome.com/icons/right-from-bracket?f=classic&amp;s=solid</t>
   </si>
 </sst>
 </file>
@@ -640,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D33"/>
+  <dimension ref="B3:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:D33"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +660,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -982,6 +991,17 @@
       </c>
       <c r="D33" s="4" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1016,8 +1036,9 @@
     <hyperlink ref="D32" r:id="rId23" xr:uid="{8845E029-3FBD-4714-B37E-75431B4A86C3}"/>
     <hyperlink ref="D31" r:id="rId24" xr:uid="{8F0CAF8B-9F27-46AA-82DD-7AA7797A3B43}"/>
     <hyperlink ref="D33" r:id="rId25" xr:uid="{2C7BCA22-ADF3-43DB-9021-C8789A457610}"/>
+    <hyperlink ref="D34" r:id="rId26" xr:uid="{1F1A467D-A3A5-4146-8C70-773F123F16DF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
better Adminlogin and LateralMenu
</commit_message>
<xml_diff>
--- a/Moqup/Iconos.xlsx
+++ b/Moqup/Iconos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GamerNest\Moqup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1566B1-79C8-436E-9B5B-158D3384C379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC54865-E110-4F9A-914D-F395BC0E2F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>MENÚ LATERAL</t>
   </si>
@@ -280,6 +280,15 @@
   </si>
   <si>
     <t>https://fontawesome.com/icons/right-from-bracket?f=classic&amp;s=solid</t>
+  </si>
+  <si>
+    <t>Flecha Atras</t>
+  </si>
+  <si>
+    <t>arrow-left</t>
+  </si>
+  <si>
+    <t>https://fontawesome.com/icons/arrow-left?f=classic&amp;s=solid</t>
   </si>
 </sst>
 </file>
@@ -649,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D34"/>
+  <dimension ref="B3:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,6 +1011,17 @@
       </c>
       <c r="D34" s="4" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1037,8 +1057,9 @@
     <hyperlink ref="D31" r:id="rId24" xr:uid="{8F0CAF8B-9F27-46AA-82DD-7AA7797A3B43}"/>
     <hyperlink ref="D33" r:id="rId25" xr:uid="{2C7BCA22-ADF3-43DB-9021-C8789A457610}"/>
     <hyperlink ref="D34" r:id="rId26" xr:uid="{1F1A467D-A3A5-4146-8C70-773F123F16DF}"/>
+    <hyperlink ref="D35" r:id="rId27" xr:uid="{67B35C53-7064-438B-9018-A31A14DCB076}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Un poco de todo
</commit_message>
<xml_diff>
--- a/Moqup/Iconos.xlsx
+++ b/Moqup/Iconos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GamerNest\Moqup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC54865-E110-4F9A-914D-F395BC0E2F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDB6F31-9BDB-46CD-938D-F39770AF6FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>MENÚ LATERAL</t>
   </si>
@@ -289,6 +289,24 @@
   </si>
   <si>
     <t>https://fontawesome.com/icons/arrow-left?f=classic&amp;s=solid</t>
+  </si>
+  <si>
+    <t>Check (True)</t>
+  </si>
+  <si>
+    <t>circle-check</t>
+  </si>
+  <si>
+    <t>https://fontawesome.com/icons/circle-check?f=classic&amp;s=regular</t>
+  </si>
+  <si>
+    <t>circle-xmark</t>
+  </si>
+  <si>
+    <t>https://fontawesome.com/icons/circle-xmark?f=classic&amp;s=regular</t>
+  </si>
+  <si>
+    <t>Check (False)</t>
   </si>
 </sst>
 </file>
@@ -658,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:D35"/>
+  <dimension ref="B3:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,6 +1040,28 @@
       </c>
       <c r="D35" s="4" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1058,8 +1098,10 @@
     <hyperlink ref="D33" r:id="rId25" xr:uid="{2C7BCA22-ADF3-43DB-9021-C8789A457610}"/>
     <hyperlink ref="D34" r:id="rId26" xr:uid="{1F1A467D-A3A5-4146-8C70-773F123F16DF}"/>
     <hyperlink ref="D35" r:id="rId27" xr:uid="{67B35C53-7064-438B-9018-A31A14DCB076}"/>
+    <hyperlink ref="D36" r:id="rId28" xr:uid="{9CD6735D-6FB2-46A9-B32A-2B902EC4477C}"/>
+    <hyperlink ref="D37" r:id="rId29" xr:uid="{D4DF8685-35A8-43AA-B52E-632E03437543}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>